<commit_message>
doc: update experiments on ResNet@CIFAR-100
</commit_message>
<xml_diff>
--- a/docs/experiments.xlsx
+++ b/docs/experiments.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1009A8-3CD6-4B90-836F-951A2F02055E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7E1E8E-968E-4FD1-BF73-EFFDF1324863}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24686" windowHeight="13149" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5400" yWindow="3900" windowWidth="24686" windowHeight="13149" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeNet@MNIST" sheetId="1" r:id="rId1"/>
@@ -1210,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35ED1B4D-1FC9-49CC-974D-A069222E61B9}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>

</xml_diff>